<commit_message>
centralizando a tela inicial
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -20,21 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Nome</t>
+    <t xml:space="preserve">Matricula</t>
   </si>
   <si>
-    <t xml:space="preserve">Idade</t>
+    <t xml:space="preserve">Valor</t>
   </si>
   <si>
-    <t xml:space="preserve">Darcio</t>
+    <t xml:space="preserve">111-x</t>
   </si>
   <si>
-    <t xml:space="preserve">Souza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oliveira</t>
+    <t xml:space="preserve">12-x</t>
   </si>
 </sst>
 </file>
@@ -108,8 +105,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -147,7 +148,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
@@ -155,7 +156,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -163,8 +164,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>4</v>
+      <c r="A4" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>35</v>

</xml_diff>

<commit_message>
completando com zeros a esquerda
</commit_message>
<xml_diff>
--- a/arquivo.xlsx
+++ b/arquivo.xlsx
@@ -22,10 +22,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Matricula</t>
+    <t xml:space="preserve">matricula</t>
   </si>
   <si>
-    <t xml:space="preserve">Valor</t>
+    <t xml:space="preserve">valor</t>
   </si>
   <si>
     <t xml:space="preserve">111-x</t>
@@ -46,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,7 +111,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,16 +135,16 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -151,7 +152,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>45</v>
       </c>
     </row>
@@ -159,7 +160,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>40</v>
       </c>
     </row>
@@ -167,7 +168,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>35</v>
       </c>
     </row>

</xml_diff>